<commit_message>
Combinaison avec acides aminés
• Le système de combinaisons a été refait en ne prenant d'abord que les acides aminés en compte
• Détermination des atomes composant les molécules candidates
• Légère modification des noms pour correspondre entre les 2 tableaux Excel

A faire :
• Conditions spéciales pour le choix des chromaphores/side chains
• Azote déjà déterminé avant les combinaisons
• Faire des combinaisons ayant plus d'une partie de molécule de chaque
</commit_message>
<xml_diff>
--- a/Pyoverdine Germain Final.xlsx
+++ b/Pyoverdine Germain Final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Projet Num\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFA3536-2F59-4C0B-84BB-C3EA135759A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4AAC8A-5857-4186-A17D-99C647BF1314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1575" windowWidth="29040" windowHeight="15840" xr2:uid="{96CE2FE7-34CF-4D1C-BF75-DAC3F69B43D4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
   <si>
     <t>Molécule</t>
   </si>
@@ -119,12 +119,6 @@
     <t>e-Lys</t>
   </si>
   <si>
-    <t>AOH-Orn</t>
-  </si>
-  <si>
-    <t>FOH-Orn</t>
-  </si>
-  <si>
     <t>cOH-Orn</t>
   </si>
   <si>
@@ -188,12 +182,6 @@
     <t>Al</t>
   </si>
   <si>
-    <t>Fe - 3H</t>
-  </si>
-  <si>
-    <t>Al - 3H</t>
-  </si>
-  <si>
     <t>Structure</t>
   </si>
   <si>
@@ -249,9 +237,6 @@
   </si>
   <si>
     <t>FoOH-Orn</t>
-  </si>
-  <si>
-    <t>Cyclisation     -H2O</t>
   </si>
   <si>
     <t>Fe(III) - 3 H+</t>
@@ -1753,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF63E52-D3EC-4971-B121-A52D5556F3D8}">
   <dimension ref="A1:BB251"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5212,7 +5197,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D16" s="19">
         <f t="shared" si="0"/>
@@ -5246,7 +5231,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="13">
@@ -5281,7 +5266,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D18" s="19">
         <f t="shared" si="0"/>
@@ -5315,7 +5300,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D19" s="19">
         <f t="shared" si="0"/>
@@ -5351,7 +5336,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D20" s="19">
         <f t="shared" si="0"/>
@@ -5385,7 +5370,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D21" s="19">
         <f t="shared" si="0"/>
@@ -5419,7 +5404,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D22" s="19">
         <f>E22*$E$2+F22*$F$2+G22*$G$2+H22*$H$2+I24*$I$2+J24*$J$2+K24*$K$2+L24*$L$2+M24*$M$2+N24*$N$2+O24*$O$2</f>
@@ -5453,7 +5438,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D23" s="19">
         <f>E23*$E$2+(F23)*$F$2+(G23)*$G$2+H23*$H$2+I22*$I$2+J22*$J$2+K22*$K$2+L22*$L$2+M22*$M$2+N22*$N$2+O22*$O$2</f>
@@ -5483,7 +5468,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="26">
@@ -5514,7 +5499,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C25">
         <f t="shared" ref="C25:C40" si="1">(D25+2*$F$2)/2</f>
@@ -5552,7 +5537,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
@@ -5590,7 +5575,7 @@
         <v>33</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
@@ -5628,7 +5613,7 @@
         <v>34</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
@@ -5666,7 +5651,7 @@
         <v>35</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
@@ -5706,7 +5691,7 @@
         <v>36</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
@@ -5744,7 +5729,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
@@ -5780,7 +5765,7 @@
         <v>38</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
@@ -5818,7 +5803,7 @@
         <v>39</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
@@ -5854,7 +5839,7 @@
         <v>40</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
@@ -5892,7 +5877,7 @@
         <v>41</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
@@ -5930,7 +5915,7 @@
         <v>42</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
@@ -5966,7 +5951,7 @@
         <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
@@ -5998,7 +5983,7 @@
         <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
@@ -6030,7 +6015,7 @@
         <v>47</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C39" s="35">
         <f t="shared" si="1"/>
@@ -6064,7 +6049,7 @@
         <v>48</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C40" s="42">
         <f t="shared" si="1"/>
@@ -13499,8 +13484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03A8ED1A-94EA-441B-9162-2FB2E8C7314C}">
   <dimension ref="A1:AU9"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13508,7 +13493,7 @@
     <row r="1" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="21"/>
       <c r="AO1" s="145" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AP1" s="146"/>
       <c r="AQ1" s="146"/>
@@ -13519,7 +13504,7 @@
     </row>
     <row r="2" spans="1:47" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="151" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F2" s="152"/>
       <c r="G2" s="152"/>
@@ -13540,11 +13525,11 @@
       <c r="V2" s="152"/>
       <c r="W2" s="153"/>
       <c r="X2" s="154" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="Y2" s="155"/>
       <c r="Z2" s="156" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AA2" s="157"/>
       <c r="AB2" s="157"/>
@@ -13552,7 +13537,7 @@
       <c r="AD2" s="157"/>
       <c r="AE2" s="158"/>
       <c r="AF2" s="159" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG2" s="160"/>
       <c r="AH2" s="160"/>
@@ -13560,7 +13545,7 @@
       <c r="AJ2" s="160"/>
       <c r="AK2" s="161"/>
       <c r="AL2" s="162" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AM2" s="163"/>
       <c r="AN2" s="15"/>
@@ -13707,16 +13692,16 @@
     </row>
     <row r="4" spans="1:47" ht="69" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="61" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D4" s="140" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E4" s="63" t="s">
         <v>16</v>
@@ -13755,94 +13740,94 @@
         <v>27</v>
       </c>
       <c r="Q4" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="R4" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="T4" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="U4" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="V4" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="W4" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="X4" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y4" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z4" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA4" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB4" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC4" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD4" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE4" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF4" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG4" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH4" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI4" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ4" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK4" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL4" s="72" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM4" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO4" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="R4" s="64" t="s">
+      <c r="AP4" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="S4" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="T4" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="U4" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="V4" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="W4" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="X4" s="66" t="s">
+      <c r="AQ4" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="Y4" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z4" s="68" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA4" s="69" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB4" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC4" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD4" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE4" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF4" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG4" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH4" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI4" s="70" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ4" s="70" t="s">
+      <c r="AR4" s="75" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS4" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT4" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="AK4" s="71" t="s">
+      <c r="AU4" s="76" t="s">
         <v>48</v>
-      </c>
-      <c r="AL4" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="AM4" s="73" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO4" s="74" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP4" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ4" s="75" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR4" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="AS4" s="75" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT4" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="AU4" s="76" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.25">
@@ -13859,7 +13844,7 @@
         <v>1213.4206499999998</v>
       </c>
       <c r="D5" s="141" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E5" s="79">
         <v>2</v>
@@ -13976,7 +13961,7 @@
         <v>1184.4678009999998</v>
       </c>
       <c r="D7" s="142" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E7" s="136">
         <v>2</v>
@@ -14093,7 +14078,7 @@
         <v>1212.4627159999998</v>
       </c>
       <c r="D9" s="141" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E9" s="79">
         <v>2</v>

</xml_diff>